<commit_message>
Added my code smells and patterns, also the Work Breakdown Structure
</commit_message>
<xml_diff>
--- a/Project/Work_breakdown_structure.xlsx
+++ b/Project/Work_breakdown_structure.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GL704G\Desktop\ES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GL704G\Desktop\ES\ESProject\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47465E4A-458D-4702-83AB-C34189D9E528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35250933-7C65-42E3-A8B3-424F9947EE87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{5FF1C84C-74F6-4503-AE0B-EA04810D9109}"/>
   </bookViews>
@@ -63,10 +63,10 @@
 1.2.3 - Provide na explanation of the rationale for identifying the design pattern.</t>
   </si>
   <si>
-    <t>1.1 Search for Code Smells.</t>
-  </si>
-  <si>
-    <t>1.2 Search for Gof Design Patterns.</t>
+    <t>1.1 Search for Code Smells</t>
+  </si>
+  <si>
+    <t>1.2 Search for Gof Design Patterns</t>
   </si>
 </sst>
 </file>
@@ -464,7 +464,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated Work_breakdown_structure and added my metrics and use case diagram with its description
</commit_message>
<xml_diff>
--- a/Project/Work_breakdown_structure.xlsx
+++ b/Project/Work_breakdown_structure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GL704G\Desktop\ES\ESProject\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35250933-7C65-42E3-A8B3-424F9947EE87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8DBD41-45A9-4650-A152-C2ED880DACE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{5FF1C84C-74F6-4503-AE0B-EA04810D9109}"/>
+    <workbookView xWindow="0" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{5FF1C84C-74F6-4503-AE0B-EA04810D9109}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve"> Level 1</t>
   </si>
@@ -67,6 +67,33 @@
   </si>
   <si>
     <t>1.2 Search for Gof Design Patterns</t>
+  </si>
+  <si>
+    <t>1.3 Use case Diagrams for the GanttProject tool</t>
+  </si>
+  <si>
+    <t>1.3.1 - Create the Use Case Diagram
+1.3.2 - Report the name, description and actors (primary and secondary)</t>
+  </si>
+  <si>
+    <t>1.4 - Codebase metrics assessment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.4.1 - Create a data file with the collected metrics
+1.4.2 - Report the collected metrics
+1.4.3 - Identification of potential trouble spots in the codebase
+1.4.4 - A short discussion on how these metrics might relate to the code smells,
+             when applicable.
+</t>
+  </si>
+  <si>
+    <t>1.5.1 - Produce two User Stories for each functionality proposed with a description of   it
+1.5.2 - Apply changes to the code with the respective Unit Tests
+1.5.3 - Create a Demo video of the two functionalaties.</t>
+  </si>
+  <si>
+    <t>1.5 - Two extensions for the
+          for ganttproject tool</t>
   </si>
 </sst>
 </file>
@@ -136,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -145,6 +172,19 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -461,16 +501,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3888A4CC-FC3B-4760-AA58-B4B792B8FF4D}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="31" customWidth="1"/>
+    <col min="2" max="2" width="42.85546875" customWidth="1"/>
     <col min="3" max="3" width="76" customWidth="1"/>
   </cols>
   <sheetData>
@@ -511,6 +551,38 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="1:6" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="80.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>